<commit_message>
test: add option tests
</commit_message>
<xml_diff>
--- a/tests/answer/case/option-car-ev-phv.test-cases.xlsx
+++ b/tests/answer/case/option-car-ev-phv.test-cases.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naoto/Documents/projects/code-for-japan/JibungotoPlanet-backend/src/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naoto/Documents/projects/code-for-japan/cfp-calc/tests/answer/case/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77ED2442-77BB-CB45-854E-CED51CD1BFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557DE129-862B-5C4A-B803-436C2B82FF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="3" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
+    <workbookView xWindow="51200" yWindow="5300" windowWidth="38400" windowHeight="23500" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
   </bookViews>
   <sheets>
-    <sheet name="answers" sheetId="24" r:id="rId1"/>
+    <sheet name="answers" sheetId="27" r:id="rId1"/>
     <sheet name="car-ev-phv01" sheetId="2" r:id="rId2"/>
     <sheet name="car-ev-phv02" sheetId="25" r:id="rId3"/>
     <sheet name="car-ev-phv03" sheetId="26" r:id="rId4"/>
@@ -1321,6 +1321,9 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1329,9 +1332,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1647,13 +1647,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F736131-A148-C54D-A8DD-F6AD54D9B482}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F9FFCF-70D8-6247-A2DE-9333649EDE7B}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
@@ -2261,19 +2261,19 @@
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="B36" s="49" t="s">
+      <c r="B36" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="C36" s="49" t="s">
+      <c r="C36" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="D36" s="49" t="s">
+      <c r="D36" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="E36" s="49" t="s">
+      <c r="E36" s="46" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2567,19 +2567,19 @@
       </c>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="49" t="s">
+      <c r="A54" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="B54" s="49" t="s">
+      <c r="B54" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="C54" s="49" t="s">
+      <c r="C54" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="D54" s="49" t="s">
+      <c r="D54" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="E54" s="49" t="s">
+      <c r="E54" s="46" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -2651,11 +2651,11 @@
       <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="47"/>
-      <c r="N1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="49"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
@@ -3449,11 +3449,11 @@
       <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="47"/>
-      <c r="N1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="49"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
@@ -4192,8 +4192,8 @@
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -4247,11 +4247,11 @@
       <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="47"/>
-      <c r="N1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="49"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">

</xml_diff>